<commit_message>
text_summ: more training. Split dataset into train/val/test splits
</commit_message>
<xml_diff>
--- a/text_summ/logs/experiment_tracker.xlsx
+++ b/text_summ/logs/experiment_tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ml_ai_portfolio\text_summ\logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52CD61C6-9364-469B-9675-95AEF320767A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48AADA8A-A799-41FD-B0CE-7ACD7048637E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{0AC54277-F8AF-4AEE-83BD-EC3E26374A59}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{0AC54277-F8AF-4AEE-83BD-EC3E26374A59}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -36,14 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="20">
   <si>
     <t>Log ID</t>
   </si>
   <si>
-    <t>000</t>
-  </si>
-  <si>
     <t>Model</t>
   </si>
   <si>
@@ -86,22 +83,19 @@
     <t>grad_accum</t>
   </si>
   <si>
-    <t>001</t>
-  </si>
-  <si>
     <t>LoRA(r=8, alpha=32, dropout=0)</t>
   </si>
   <si>
-    <t>002</t>
-  </si>
-  <si>
-    <t>003</t>
-  </si>
-  <si>
-    <t>004</t>
-  </si>
-  <si>
     <t>early stopping</t>
+  </si>
+  <si>
+    <t>Index</t>
+  </si>
+  <si>
+    <t>LoRA(r=16, alpha=32, dropout=0)</t>
+  </si>
+  <si>
+    <t>LoRA(r=8, alpha=64, dropout=0)</t>
   </si>
 </sst>
 </file>
@@ -475,253 +469,788 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87974732-3FB0-4A1F-B867-3637CD3F37C3}">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:M37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="L1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="str">
+        <f>CONCATENATE("00",A2)</f>
+        <v>000</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2">
+        <v>5</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>2</v>
+      </c>
+      <c r="J2">
+        <v>4</v>
+      </c>
+      <c r="K2" s="1">
+        <v>5.0000000000000002E-5</v>
+      </c>
+      <c r="L2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>A2+1</f>
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="str">
+        <f t="shared" ref="B3:B37" si="0">CONCATENATE("00",A3)</f>
+        <v>001</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3">
+        <v>5</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <v>4</v>
+      </c>
+      <c r="K3" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="L3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f t="shared" ref="A4:A37" si="1">A3+1</f>
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>002</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <v>5</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <v>2</v>
+      </c>
+      <c r="J4">
+        <v>4</v>
+      </c>
+      <c r="K4" s="1">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="L4" t="s">
+        <v>10</v>
+      </c>
+      <c r="M4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>003</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5">
+        <v>5</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <v>4</v>
+      </c>
+      <c r="K5" s="1">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="L5" t="s">
+        <v>10</v>
+      </c>
+      <c r="M5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>004</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="H6">
+        <v>2</v>
+      </c>
+      <c r="I6">
+        <v>2</v>
+      </c>
+      <c r="J6">
+        <v>4</v>
+      </c>
+      <c r="K6" s="1">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="L6" t="s">
+        <v>10</v>
+      </c>
+      <c r="M6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>005</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7">
+        <v>5</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="I7">
+        <v>2</v>
+      </c>
+      <c r="J7">
+        <v>4</v>
+      </c>
+      <c r="K7" s="1">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="L7" t="s">
+        <v>10</v>
+      </c>
+      <c r="M7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>006</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8">
+        <v>5</v>
+      </c>
+      <c r="H8">
+        <v>2</v>
+      </c>
+      <c r="I8">
+        <v>2</v>
+      </c>
+      <c r="J8">
+        <v>4</v>
+      </c>
+      <c r="K8" s="1">
+        <v>3.2000000000000002E-3</v>
+      </c>
+      <c r="L8" t="s">
+        <v>10</v>
+      </c>
+      <c r="M8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>007</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>008</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>009</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="B12" s="2" t="str">
+        <f>CONCATENATE("0",A12)</f>
+        <v>010</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="B13" s="2" t="str">
+        <f t="shared" ref="B13:B37" si="2">CONCATENATE("0",A13)</f>
+        <v>011</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="G1" t="s">
+      <c r="B14" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>012</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="H1" t="s">
+      <c r="B15" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>013</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="I1" t="s">
+      <c r="B16" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>014</v>
+      </c>
+      <c r="C16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
         <v>15</v>
       </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="E16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G16">
+        <v>5</v>
+      </c>
+      <c r="H16">
+        <v>2</v>
+      </c>
+      <c r="I16">
+        <v>2</v>
+      </c>
+      <c r="J16">
+        <v>2</v>
+      </c>
+      <c r="K16" s="1">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="L16" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="B17" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>015</v>
+      </c>
+      <c r="C17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17">
+        <v>5</v>
+      </c>
+      <c r="H17">
+        <v>2</v>
+      </c>
+      <c r="I17">
+        <v>2</v>
+      </c>
+      <c r="J17">
+        <v>8</v>
+      </c>
+      <c r="K17" s="1">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="L17" t="s">
+        <v>10</v>
+      </c>
+      <c r="M17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="B18" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>016</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="B19" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>017</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="B20" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>018</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="B21" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>019</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="B22" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>020</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B23" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>021</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="B24" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>022</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="B25" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>023</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="B26" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>024</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="B27" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>025</v>
+      </c>
+      <c r="C27" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" t="s">
+        <v>18</v>
+      </c>
+      <c r="E27" t="s">
+        <v>4</v>
+      </c>
+      <c r="F27" t="s">
+        <v>4</v>
+      </c>
+      <c r="G27">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H27">
+        <v>2</v>
+      </c>
+      <c r="I27">
+        <v>2</v>
+      </c>
+      <c r="J27">
+        <v>4</v>
+      </c>
+      <c r="K27" s="1">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="L27" t="s">
+        <v>10</v>
+      </c>
+      <c r="M27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="B28" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>026</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="B29" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>027</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="B30" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>028</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="B31" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>029</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="B32" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>030</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="B33" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>031</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="B34" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>032</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="B35" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>033</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="B36" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>034</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="B37" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>035</v>
+      </c>
+      <c r="C37" t="s">
+        <v>2</v>
+      </c>
+      <c r="D37" t="s">
+        <v>19</v>
+      </c>
+      <c r="E37" t="s">
+        <v>4</v>
+      </c>
+      <c r="F37" t="s">
+        <v>4</v>
+      </c>
+      <c r="G37">
         <v>5</v>
       </c>
-      <c r="F2">
-        <v>5</v>
-      </c>
-      <c r="G2">
-        <v>2</v>
-      </c>
-      <c r="H2">
-        <v>2</v>
-      </c>
-      <c r="I2">
-        <v>4</v>
-      </c>
-      <c r="J2" s="1">
-        <v>5.0000000000000002E-5</v>
-      </c>
-      <c r="K2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3">
-        <v>5</v>
-      </c>
-      <c r="G3">
-        <v>2</v>
-      </c>
-      <c r="H3">
-        <v>2</v>
-      </c>
-      <c r="I3">
-        <v>4</v>
-      </c>
-      <c r="J3" s="1">
-        <v>1E-4</v>
-      </c>
-      <c r="K3" t="s">
-        <v>11</v>
-      </c>
-      <c r="L3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4">
-        <v>5</v>
-      </c>
-      <c r="G4">
-        <v>2</v>
-      </c>
-      <c r="H4">
-        <v>2</v>
-      </c>
-      <c r="I4">
-        <v>4</v>
-      </c>
-      <c r="J4" s="1">
-        <v>2.0000000000000001E-4</v>
-      </c>
-      <c r="K4" t="s">
-        <v>11</v>
-      </c>
-      <c r="L4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5">
-        <v>5</v>
-      </c>
-      <c r="G5">
-        <v>2</v>
-      </c>
-      <c r="H5">
-        <v>2</v>
-      </c>
-      <c r="I5">
-        <v>4</v>
-      </c>
-      <c r="J5" s="1">
-        <v>4.0000000000000002E-4</v>
-      </c>
-      <c r="K5" t="s">
-        <v>11</v>
-      </c>
-      <c r="L5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6">
-        <v>5</v>
-      </c>
-      <c r="G6">
-        <v>2</v>
-      </c>
-      <c r="H6">
-        <v>2</v>
-      </c>
-      <c r="I6">
-        <v>4</v>
-      </c>
-      <c r="J6" s="1">
+      <c r="H37">
+        <v>2</v>
+      </c>
+      <c r="I37">
+        <v>2</v>
+      </c>
+      <c r="J37">
+        <v>4</v>
+      </c>
+      <c r="K37" s="1">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="K6" t="s">
-        <v>11</v>
-      </c>
-      <c r="L6" t="s">
-        <v>7</v>
+      <c r="L37" t="s">
+        <v>10</v>
+      </c>
+      <c r="M37" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
text_summ: unfroze lm_head and model is now overfitting
</commit_message>
<xml_diff>
--- a/text_summ/logs/experiment_tracker.xlsx
+++ b/text_summ/logs/experiment_tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ml_ai_portfolio\text_summ\logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48AADA8A-A799-41FD-B0CE-7ACD7048637E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0704DD3-29D0-442F-9507-AFB92FBC6431}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{0AC54277-F8AF-4AEE-83BD-EC3E26374A59}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{0AC54277-F8AF-4AEE-83BD-EC3E26374A59}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="34">
   <si>
     <t>Log ID</t>
   </si>
@@ -96,6 +96,48 @@
   </si>
   <si>
     <t>LoRA(r=8, alpha=64, dropout=0)</t>
+  </si>
+  <si>
+    <t>LoRA(r=32, alpha=32, dropout=0)</t>
+  </si>
+  <si>
+    <t>Trained?</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>LoRA(r=4, alpha=32, dropout=0)</t>
+  </si>
+  <si>
+    <t>LoRA(r=2, alpha=32, dropout=0)</t>
+  </si>
+  <si>
+    <t>LoRA(r=32, alpha=64, dropout=0)</t>
+  </si>
+  <si>
+    <t>LoRA(r=32, alpha=128, dropout=0)</t>
+  </si>
+  <si>
+    <t>LoRA(r=64, alpha=128, dropout=0)</t>
+  </si>
+  <si>
+    <t>5a</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>unfreeze lm head</t>
+  </si>
+  <si>
+    <t>LoRA(r=8, alpha=32, dropout=0.1)</t>
+  </si>
+  <si>
+    <t>lm_dropout</t>
+  </si>
+  <si>
+    <t>weight_decay</t>
   </si>
 </sst>
 </file>
@@ -469,10 +511,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87974732-3FB0-4A1F-B867-3637CD3F37C3}">
-  <dimension ref="A1:M37"/>
+  <dimension ref="A1:Q72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,17 +523,20 @@
     <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -504,34 +550,46 @@
         <v>7</v>
       </c>
       <c r="E1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>12</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>13</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>14</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -545,41 +603,44 @@
       <c r="D2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2">
+      <c r="G2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2">
         <v>5</v>
       </c>
-      <c r="H2">
-        <v>2</v>
-      </c>
-      <c r="I2">
-        <v>2</v>
-      </c>
       <c r="J2">
-        <v>4</v>
-      </c>
-      <c r="K2" s="1">
+        <v>2</v>
+      </c>
+      <c r="K2">
+        <v>2</v>
+      </c>
+      <c r="L2">
+        <v>4</v>
+      </c>
+      <c r="M2" s="1">
         <v>5.0000000000000002E-5</v>
       </c>
-      <c r="L2" t="s">
-        <v>10</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
+        <v>10</v>
+      </c>
+      <c r="O2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+1</f>
         <v>1</v>
       </c>
       <c r="B3" s="2" t="str">
-        <f t="shared" ref="B3:B37" si="0">CONCATENATE("00",A3)</f>
+        <f t="shared" ref="B3:B12" si="0">CONCATENATE("00",A3)</f>
         <v>001</v>
       </c>
       <c r="C3" t="s">
@@ -588,37 +649,40 @@
       <c r="D3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3">
+      <c r="G3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3">
         <v>5</v>
       </c>
-      <c r="H3">
-        <v>2</v>
-      </c>
-      <c r="I3">
-        <v>2</v>
-      </c>
       <c r="J3">
-        <v>4</v>
-      </c>
-      <c r="K3" s="1">
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
+      <c r="L3">
+        <v>4</v>
+      </c>
+      <c r="M3" s="1">
         <v>1E-4</v>
       </c>
-      <c r="L3" t="s">
-        <v>10</v>
-      </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
+        <v>10</v>
+      </c>
+      <c r="O3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A37" si="1">A3+1</f>
+        <f t="shared" ref="A4:A67" si="1">A3+1</f>
         <v>2</v>
       </c>
       <c r="B4" s="2" t="str">
@@ -631,35 +695,38 @@
       <c r="D4" t="s">
         <v>15</v>
       </c>
-      <c r="E4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4">
+      <c r="G4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I4">
         <v>5</v>
       </c>
-      <c r="H4">
-        <v>2</v>
-      </c>
-      <c r="I4">
-        <v>2</v>
-      </c>
       <c r="J4">
-        <v>4</v>
-      </c>
-      <c r="K4" s="1">
+        <v>2</v>
+      </c>
+      <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4">
+        <v>4</v>
+      </c>
+      <c r="M4" s="1">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="L4" t="s">
-        <v>10</v>
-      </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
+        <v>10</v>
+      </c>
+      <c r="O4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="1"/>
         <v>3</v>
@@ -674,35 +741,38 @@
       <c r="D5" t="s">
         <v>15</v>
       </c>
-      <c r="E5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5">
+      <c r="G5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5">
         <v>5</v>
       </c>
-      <c r="H5">
-        <v>2</v>
-      </c>
-      <c r="I5">
-        <v>2</v>
-      </c>
       <c r="J5">
-        <v>4</v>
-      </c>
-      <c r="K5" s="1">
+        <v>2</v>
+      </c>
+      <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="L5">
+        <v>4</v>
+      </c>
+      <c r="M5" s="1">
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="L5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
+        <v>10</v>
+      </c>
+      <c r="O5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -717,35 +787,38 @@
       <c r="D6" t="s">
         <v>15</v>
       </c>
-      <c r="E6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G6">
+      <c r="G6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6">
         <v>5</v>
       </c>
-      <c r="H6">
-        <v>2</v>
-      </c>
-      <c r="I6">
-        <v>2</v>
-      </c>
       <c r="J6">
-        <v>4</v>
-      </c>
-      <c r="K6" s="1">
+        <v>2</v>
+      </c>
+      <c r="K6">
+        <v>2</v>
+      </c>
+      <c r="L6">
+        <v>4</v>
+      </c>
+      <c r="M6" s="1">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="L6" t="s">
-        <v>10</v>
-      </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
+        <v>10</v>
+      </c>
+      <c r="O6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -760,42 +833,44 @@
       <c r="D7" t="s">
         <v>15</v>
       </c>
-      <c r="E7" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" t="s">
-        <v>4</v>
-      </c>
-      <c r="G7">
+      <c r="G7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7">
         <v>5</v>
       </c>
-      <c r="H7">
-        <v>2</v>
-      </c>
-      <c r="I7">
-        <v>2</v>
-      </c>
       <c r="J7">
-        <v>4</v>
-      </c>
-      <c r="K7" s="1">
+        <v>2</v>
+      </c>
+      <c r="K7">
+        <v>2</v>
+      </c>
+      <c r="L7">
+        <v>4</v>
+      </c>
+      <c r="M7" s="1">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="L7" t="s">
-        <v>10</v>
-      </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
+        <v>10</v>
+      </c>
+      <c r="O7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <f t="shared" si="1"/>
-        <v>6</v>
+      <c r="Q7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="B8" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>006</v>
+        <v>005a</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
@@ -803,155 +878,164 @@
       <c r="D8" t="s">
         <v>15</v>
       </c>
-      <c r="E8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F8" t="s">
-        <v>4</v>
-      </c>
-      <c r="G8">
+      <c r="G8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I8">
         <v>5</v>
       </c>
-      <c r="H8">
-        <v>2</v>
-      </c>
-      <c r="I8">
-        <v>2</v>
-      </c>
       <c r="J8">
-        <v>4</v>
-      </c>
-      <c r="K8" s="1">
-        <v>3.2000000000000002E-3</v>
-      </c>
-      <c r="L8" t="s">
-        <v>10</v>
-      </c>
-      <c r="M8" t="s">
+        <v>2</v>
+      </c>
+      <c r="K8">
+        <v>2</v>
+      </c>
+      <c r="L8">
+        <v>4</v>
+      </c>
+      <c r="M8" s="1">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="N8" t="s">
+        <v>10</v>
+      </c>
+      <c r="O8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P8" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f t="shared" si="1"/>
-        <v>7</v>
+        <f>A7+1</f>
+        <v>6</v>
       </c>
       <c r="B9" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>007</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+        <v>006</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" t="s">
+        <v>4</v>
+      </c>
+      <c r="I9">
+        <v>5</v>
+      </c>
+      <c r="J9">
+        <v>2</v>
+      </c>
+      <c r="K9">
+        <v>2</v>
+      </c>
+      <c r="L9">
+        <v>4</v>
+      </c>
+      <c r="M9" s="1">
+        <v>3.2000000000000002E-3</v>
+      </c>
+      <c r="N9" t="s">
+        <v>10</v>
+      </c>
+      <c r="O9" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>008</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+        <v>007</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" s="2" t="str">
         <f t="shared" si="0"/>
+        <v>008</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="B12" s="2" t="str">
+        <f t="shared" si="0"/>
         <v>009</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="B12" s="2" t="str">
-        <f>CONCATENATE("0",A12)</f>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="B13" s="2" t="str">
+        <f>CONCATENATE("0",A13)</f>
         <v>010</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="B13" s="2" t="str">
-        <f t="shared" ref="B13:B37" si="2">CONCATENATE("0",A13)</f>
+      <c r="B14" s="2" t="str">
+        <f t="shared" ref="B14:B38" si="2">CONCATENATE("0",A14)</f>
         <v>011</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="B14" s="2" t="str">
+      <c r="B15" s="2" t="str">
         <f t="shared" si="2"/>
         <v>012</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="B15" s="2" t="str">
+      <c r="B16" s="2" t="str">
         <f t="shared" si="2"/>
         <v>013</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="B16" s="2" t="str">
+      <c r="B17" s="2" t="str">
         <f t="shared" si="2"/>
         <v>014</v>
-      </c>
-      <c r="C16" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" t="s">
-        <v>4</v>
-      </c>
-      <c r="F16" t="s">
-        <v>4</v>
-      </c>
-      <c r="G16">
-        <v>5</v>
-      </c>
-      <c r="H16">
-        <v>2</v>
-      </c>
-      <c r="I16">
-        <v>2</v>
-      </c>
-      <c r="J16">
-        <v>2</v>
-      </c>
-      <c r="K16" s="1">
-        <v>1.6000000000000001E-3</v>
-      </c>
-      <c r="L16" t="s">
-        <v>10</v>
-      </c>
-      <c r="M16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-      <c r="B17" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>015</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
@@ -959,298 +1043,978 @@
       <c r="D17" t="s">
         <v>15</v>
       </c>
-      <c r="E17" t="s">
-        <v>4</v>
-      </c>
-      <c r="F17" t="s">
-        <v>4</v>
-      </c>
-      <c r="G17">
+      <c r="G17" t="s">
+        <v>4</v>
+      </c>
+      <c r="H17" t="s">
+        <v>4</v>
+      </c>
+      <c r="I17">
         <v>5</v>
       </c>
-      <c r="H17">
-        <v>2</v>
-      </c>
-      <c r="I17">
-        <v>2</v>
-      </c>
       <c r="J17">
+        <v>2</v>
+      </c>
+      <c r="K17">
+        <v>2</v>
+      </c>
+      <c r="L17">
+        <v>2</v>
+      </c>
+      <c r="M17" s="1">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="N17" t="s">
+        <v>10</v>
+      </c>
+      <c r="O17" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="B18" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>015</v>
+      </c>
+      <c r="C18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>15</v>
+      </c>
+      <c r="G18" t="s">
+        <v>4</v>
+      </c>
+      <c r="H18" t="s">
+        <v>4</v>
+      </c>
+      <c r="I18">
+        <v>5</v>
+      </c>
+      <c r="J18">
+        <v>2</v>
+      </c>
+      <c r="K18">
+        <v>2</v>
+      </c>
+      <c r="L18">
         <v>8</v>
       </c>
-      <c r="K17" s="1">
+      <c r="M18" s="1">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="L17" t="s">
-        <v>10</v>
-      </c>
-      <c r="M17" t="s">
+      <c r="N18" t="s">
+        <v>10</v>
+      </c>
+      <c r="O18" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="Q18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="B18" s="2" t="str">
+      <c r="B19" s="2" t="str">
         <f t="shared" si="2"/>
         <v>016</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="B19" s="2" t="str">
+      <c r="B20" s="2" t="str">
         <f t="shared" si="2"/>
         <v>017</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="B20" s="2" t="str">
+      <c r="B21" s="2" t="str">
         <f t="shared" si="2"/>
         <v>018</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="B21" s="2" t="str">
+      <c r="B22" s="2" t="str">
         <f t="shared" si="2"/>
         <v>019</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="B22" s="2" t="str">
+      <c r="B23" s="2" t="str">
         <f t="shared" si="2"/>
         <v>020</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="B23" s="2" t="str">
+      <c r="B24" s="2" t="str">
         <f t="shared" si="2"/>
         <v>021</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="B24" s="2" t="str">
+      <c r="B25" s="2" t="str">
         <f t="shared" si="2"/>
         <v>022</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="B25" s="2" t="str">
+      <c r="B26" s="2" t="str">
         <f t="shared" si="2"/>
         <v>023</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <f t="shared" si="1"/>
+      <c r="C26" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="2" t="str">
+      <c r="G26" t="s">
+        <v>4</v>
+      </c>
+      <c r="H26" t="s">
+        <v>4</v>
+      </c>
+      <c r="I26">
+        <v>5</v>
+      </c>
+      <c r="J26">
+        <v>2</v>
+      </c>
+      <c r="K26">
+        <v>2</v>
+      </c>
+      <c r="L26">
+        <v>4</v>
+      </c>
+      <c r="M26" s="1">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="N26" t="s">
+        <v>10</v>
+      </c>
+      <c r="O26" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="B27" s="2" t="str">
         <f t="shared" si="2"/>
         <v>024</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27">
+      <c r="C27" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" t="s">
+        <v>23</v>
+      </c>
+      <c r="G27" t="s">
+        <v>4</v>
+      </c>
+      <c r="H27" t="s">
+        <v>4</v>
+      </c>
+      <c r="I27">
+        <v>5</v>
+      </c>
+      <c r="J27">
+        <v>2</v>
+      </c>
+      <c r="K27">
+        <v>2</v>
+      </c>
+      <c r="L27">
+        <v>4</v>
+      </c>
+      <c r="M27" s="1">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="N27" t="s">
+        <v>10</v>
+      </c>
+      <c r="O27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A28">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="B27" s="2" t="str">
+      <c r="B28" s="2" t="str">
         <f t="shared" si="2"/>
         <v>025</v>
       </c>
-      <c r="C27" t="s">
-        <v>2</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="C28" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28" t="s">
         <v>18</v>
       </c>
-      <c r="E27" t="s">
-        <v>4</v>
-      </c>
-      <c r="F27" t="s">
-        <v>4</v>
-      </c>
-      <c r="G27">
+      <c r="G28" t="s">
+        <v>4</v>
+      </c>
+      <c r="H28" t="s">
+        <v>4</v>
+      </c>
+      <c r="I28">
         <v>5</v>
       </c>
-      <c r="H27">
-        <v>2</v>
-      </c>
-      <c r="I27">
-        <v>2</v>
-      </c>
-      <c r="J27">
-        <v>4</v>
-      </c>
-      <c r="K27" s="1">
+      <c r="J28">
+        <v>2</v>
+      </c>
+      <c r="K28">
+        <v>2</v>
+      </c>
+      <c r="L28">
+        <v>4</v>
+      </c>
+      <c r="M28" s="1">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="L27" t="s">
-        <v>10</v>
-      </c>
-      <c r="M27" t="s">
+      <c r="N28" t="s">
+        <v>10</v>
+      </c>
+      <c r="O28" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28">
+      <c r="Q28" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A29">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="B28" s="2" t="str">
+      <c r="B29" s="2" t="str">
         <f t="shared" si="2"/>
         <v>026</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29">
+      <c r="C29" t="s">
+        <v>2</v>
+      </c>
+      <c r="D29" t="s">
+        <v>20</v>
+      </c>
+      <c r="G29" t="s">
+        <v>4</v>
+      </c>
+      <c r="H29" t="s">
+        <v>4</v>
+      </c>
+      <c r="I29">
+        <v>5</v>
+      </c>
+      <c r="J29">
+        <v>2</v>
+      </c>
+      <c r="K29">
+        <v>2</v>
+      </c>
+      <c r="L29">
+        <v>4</v>
+      </c>
+      <c r="M29" s="1">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="N29" t="s">
+        <v>10</v>
+      </c>
+      <c r="O29" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A30">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="B29" s="2" t="str">
+      <c r="B30" s="2" t="str">
         <f t="shared" si="2"/>
         <v>027</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A31">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="B30" s="2" t="str">
+      <c r="B31" s="2" t="str">
         <f t="shared" si="2"/>
         <v>028</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A32">
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="B31" s="2" t="str">
+      <c r="B32" s="2" t="str">
         <f t="shared" si="2"/>
         <v>029</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A33">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="B32" s="2" t="str">
+      <c r="B33" s="2" t="str">
         <f t="shared" si="2"/>
         <v>030</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A34">
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
-      <c r="B33" s="2" t="str">
+      <c r="B34" s="2" t="str">
         <f t="shared" si="2"/>
         <v>031</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A35">
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="B34" s="2" t="str">
+      <c r="B35" s="2" t="str">
         <f t="shared" si="2"/>
         <v>032</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A36">
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="B35" s="2" t="str">
+      <c r="B36" s="2" t="str">
         <f t="shared" si="2"/>
         <v>033</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A37">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="B36" s="2" t="str">
+      <c r="B37" s="2" t="str">
         <f t="shared" si="2"/>
         <v>034</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A38">
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="B37" s="2" t="str">
+      <c r="B38" s="2" t="str">
         <f t="shared" si="2"/>
         <v>035</v>
       </c>
-      <c r="C37" t="s">
-        <v>2</v>
-      </c>
-      <c r="D37" t="s">
+      <c r="C38" t="s">
+        <v>2</v>
+      </c>
+      <c r="D38" t="s">
         <v>19</v>
       </c>
-      <c r="E37" t="s">
-        <v>4</v>
-      </c>
-      <c r="F37" t="s">
-        <v>4</v>
-      </c>
-      <c r="G37">
+      <c r="G38" t="s">
+        <v>4</v>
+      </c>
+      <c r="H38" t="s">
+        <v>4</v>
+      </c>
+      <c r="I38">
         <v>5</v>
       </c>
-      <c r="H37">
-        <v>2</v>
-      </c>
-      <c r="I37">
-        <v>2</v>
-      </c>
-      <c r="J37">
-        <v>4</v>
-      </c>
-      <c r="K37" s="1">
+      <c r="J38">
+        <v>2</v>
+      </c>
+      <c r="K38">
+        <v>2</v>
+      </c>
+      <c r="L38">
+        <v>4</v>
+      </c>
+      <c r="M38" s="1">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="L37" t="s">
-        <v>10</v>
-      </c>
-      <c r="M37" t="s">
+      <c r="N38" t="s">
+        <v>10</v>
+      </c>
+      <c r="O38" t="s">
         <v>6</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="B39" s="2" t="str">
+        <f t="shared" ref="B39:B53" si="3">CONCATENATE("0",A39)</f>
+        <v>036</v>
+      </c>
+      <c r="C39" t="s">
+        <v>2</v>
+      </c>
+      <c r="D39" t="s">
+        <v>25</v>
+      </c>
+      <c r="G39" t="s">
+        <v>4</v>
+      </c>
+      <c r="H39" t="s">
+        <v>4</v>
+      </c>
+      <c r="I39">
+        <v>5</v>
+      </c>
+      <c r="J39">
+        <v>2</v>
+      </c>
+      <c r="K39">
+        <v>2</v>
+      </c>
+      <c r="L39">
+        <v>4</v>
+      </c>
+      <c r="M39" s="1">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="N39" t="s">
+        <v>10</v>
+      </c>
+      <c r="O39" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="B40" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>037</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="B41" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>038</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="B42" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>039</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="B43" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>040</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="B44" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>041</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="B45" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>042</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="B46" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>043</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="B47" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>044</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="B48" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>045</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="B49" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>046</v>
+      </c>
+      <c r="C49" t="s">
+        <v>2</v>
+      </c>
+      <c r="D49" t="s">
+        <v>26</v>
+      </c>
+      <c r="G49" t="s">
+        <v>4</v>
+      </c>
+      <c r="H49" t="s">
+        <v>4</v>
+      </c>
+      <c r="I49">
+        <v>5</v>
+      </c>
+      <c r="J49">
+        <v>2</v>
+      </c>
+      <c r="K49">
+        <v>2</v>
+      </c>
+      <c r="L49">
+        <v>4</v>
+      </c>
+      <c r="M49" s="1">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="N49" t="s">
+        <v>10</v>
+      </c>
+      <c r="O49" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="B50" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>047</v>
+      </c>
+      <c r="C50" t="s">
+        <v>2</v>
+      </c>
+      <c r="D50" t="s">
+        <v>27</v>
+      </c>
+      <c r="G50" t="s">
+        <v>4</v>
+      </c>
+      <c r="H50" t="s">
+        <v>4</v>
+      </c>
+      <c r="I50">
+        <v>5</v>
+      </c>
+      <c r="J50">
+        <v>2</v>
+      </c>
+      <c r="K50">
+        <v>2</v>
+      </c>
+      <c r="L50">
+        <v>4</v>
+      </c>
+      <c r="M50" s="1">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="N50" t="s">
+        <v>10</v>
+      </c>
+      <c r="O50" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="B51" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>048</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="B52" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>049</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="B53" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>050</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <f t="shared" si="1"/>
+        <v>51</v>
+      </c>
+      <c r="B54" s="2" t="str">
+        <f t="shared" ref="B54:B72" si="4">CONCATENATE("0",A54)</f>
+        <v>051</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
+      <c r="B55" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>052</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <f t="shared" si="1"/>
+        <v>53</v>
+      </c>
+      <c r="B56" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>053</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
+      <c r="B57" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>054</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+      <c r="B58" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>055</v>
+      </c>
+      <c r="C58" t="s">
+        <v>2</v>
+      </c>
+      <c r="D58" t="s">
+        <v>31</v>
+      </c>
+      <c r="G58" t="s">
+        <v>4</v>
+      </c>
+      <c r="H58" t="s">
+        <v>4</v>
+      </c>
+      <c r="I58">
+        <v>10</v>
+      </c>
+      <c r="J58">
+        <v>2</v>
+      </c>
+      <c r="K58">
+        <v>2</v>
+      </c>
+      <c r="L58">
+        <v>4</v>
+      </c>
+      <c r="M58" s="1">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="N58" t="s">
+        <v>10</v>
+      </c>
+      <c r="O58" t="s">
+        <v>6</v>
+      </c>
+      <c r="P58" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <f t="shared" si="1"/>
+        <v>56</v>
+      </c>
+      <c r="B59" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>056</v>
+      </c>
+      <c r="C59" t="s">
+        <v>2</v>
+      </c>
+      <c r="D59" t="s">
+        <v>31</v>
+      </c>
+      <c r="E59">
+        <v>0.1</v>
+      </c>
+      <c r="G59" t="s">
+        <v>4</v>
+      </c>
+      <c r="H59" t="s">
+        <v>4</v>
+      </c>
+      <c r="I59">
+        <v>10</v>
+      </c>
+      <c r="J59">
+        <v>2</v>
+      </c>
+      <c r="K59">
+        <v>2</v>
+      </c>
+      <c r="L59">
+        <v>4</v>
+      </c>
+      <c r="M59" s="1">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="N59" t="s">
+        <v>10</v>
+      </c>
+      <c r="O59" t="s">
+        <v>6</v>
+      </c>
+      <c r="P59" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <f t="shared" si="1"/>
+        <v>57</v>
+      </c>
+      <c r="B60" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>057</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <f t="shared" si="1"/>
+        <v>58</v>
+      </c>
+      <c r="B61" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>058</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <f t="shared" si="1"/>
+        <v>59</v>
+      </c>
+      <c r="B62" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>059</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="B63" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>060</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <f t="shared" si="1"/>
+        <v>61</v>
+      </c>
+      <c r="B64" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>061</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <f t="shared" si="1"/>
+        <v>62</v>
+      </c>
+      <c r="B65" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>062</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <f t="shared" si="1"/>
+        <v>63</v>
+      </c>
+      <c r="B66" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>063</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <f t="shared" si="1"/>
+        <v>64</v>
+      </c>
+      <c r="B67" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>064</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <f t="shared" ref="A68:A72" si="5">A67+1</f>
+        <v>65</v>
+      </c>
+      <c r="B68" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>065</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <f t="shared" si="5"/>
+        <v>66</v>
+      </c>
+      <c r="B69" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>066</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <f t="shared" si="5"/>
+        <v>67</v>
+      </c>
+      <c r="B70" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>067</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <f t="shared" si="5"/>
+        <v>68</v>
+      </c>
+      <c r="B71" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>068</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <f t="shared" si="5"/>
+        <v>69</v>
+      </c>
+      <c r="B72" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>069</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
text_summ: dropout and weight decay experiments
</commit_message>
<xml_diff>
--- a/text_summ/logs/experiment_tracker.xlsx
+++ b/text_summ/logs/experiment_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ml_ai_portfolio\text_summ\logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0704DD3-29D0-442F-9507-AFB92FBC6431}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5672399F-D00E-447F-9F32-63149734CC65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{0AC54277-F8AF-4AEE-83BD-EC3E26374A59}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="45">
   <si>
     <t>Log ID</t>
   </si>
@@ -86,9 +86,6 @@
     <t>LoRA(r=8, alpha=32, dropout=0)</t>
   </si>
   <si>
-    <t>early stopping</t>
-  </si>
-  <si>
     <t>Index</t>
   </si>
   <si>
@@ -131,13 +128,49 @@
     <t>unfreeze lm head</t>
   </si>
   <si>
-    <t>LoRA(r=8, alpha=32, dropout=0.1)</t>
-  </si>
-  <si>
-    <t>lm_dropout</t>
-  </si>
-  <si>
     <t>weight_decay</t>
+  </si>
+  <si>
+    <t>BART dropout</t>
+  </si>
+  <si>
+    <t>Early stopping</t>
+  </si>
+  <si>
+    <t>dropout=0.1, act=0.1, att=0.1</t>
+  </si>
+  <si>
+    <t>dropout=0.2, act=0.1, att=0.1</t>
+  </si>
+  <si>
+    <t>dropout=0.9, act=0.1, att=0.1</t>
+  </si>
+  <si>
+    <t>dropout=0.4, act=0.1, att=0.1</t>
+  </si>
+  <si>
+    <t>5a-10</t>
+  </si>
+  <si>
+    <t>5-10</t>
+  </si>
+  <si>
+    <t>55a</t>
+  </si>
+  <si>
+    <t>dropout=0.2, act=0.2, att=0.1</t>
+  </si>
+  <si>
+    <t>55b</t>
+  </si>
+  <si>
+    <t>55c</t>
+  </si>
+  <si>
+    <t>dropout=0.2, act=0.1, att=0.2</t>
+  </si>
+  <si>
+    <t>dropout=0.2, act=0.2, att=0.2</t>
   </si>
 </sst>
 </file>
@@ -511,19 +544,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87974732-3FB0-4A1F-B867-3637CD3F37C3}">
-  <dimension ref="A1:Q72"/>
+  <dimension ref="A1:Q84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F59" sqref="F59"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q79" sqref="Q79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
@@ -538,7 +571,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -550,10 +583,10 @@
         <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
@@ -580,13 +613,13 @@
         <v>9</v>
       </c>
       <c r="O1" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="P1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Q1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -603,6 +636,9 @@
       <c r="D2" t="s">
         <v>15</v>
       </c>
+      <c r="E2" t="s">
+        <v>33</v>
+      </c>
       <c r="G2" t="s">
         <v>4</v>
       </c>
@@ -631,7 +667,7 @@
         <v>6</v>
       </c>
       <c r="Q2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -640,7 +676,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="str">
-        <f t="shared" ref="B3:B12" si="0">CONCATENATE("00",A3)</f>
+        <f t="shared" ref="B3:B14" si="0">CONCATENATE("00",A3)</f>
         <v>001</v>
       </c>
       <c r="C3" t="s">
@@ -649,6 +685,9 @@
       <c r="D3" t="s">
         <v>15</v>
       </c>
+      <c r="E3" t="s">
+        <v>33</v>
+      </c>
       <c r="G3" t="s">
         <v>4</v>
       </c>
@@ -677,12 +716,12 @@
         <v>6</v>
       </c>
       <c r="Q3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A67" si="1">A3+1</f>
+        <f t="shared" ref="A4:A72" si="1">A3+1</f>
         <v>2</v>
       </c>
       <c r="B4" s="2" t="str">
@@ -695,6 +734,9 @@
       <c r="D4" t="s">
         <v>15</v>
       </c>
+      <c r="E4" t="s">
+        <v>33</v>
+      </c>
       <c r="G4" t="s">
         <v>4</v>
       </c>
@@ -723,7 +765,7 @@
         <v>6</v>
       </c>
       <c r="Q4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -741,6 +783,9 @@
       <c r="D5" t="s">
         <v>15</v>
       </c>
+      <c r="E5" t="s">
+        <v>33</v>
+      </c>
       <c r="G5" t="s">
         <v>4</v>
       </c>
@@ -769,7 +814,7 @@
         <v>6</v>
       </c>
       <c r="Q5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -787,6 +832,9 @@
       <c r="D6" t="s">
         <v>15</v>
       </c>
+      <c r="E6" t="s">
+        <v>33</v>
+      </c>
       <c r="G6" t="s">
         <v>4</v>
       </c>
@@ -815,7 +863,7 @@
         <v>6</v>
       </c>
       <c r="Q6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -833,6 +881,9 @@
       <c r="D7" t="s">
         <v>15</v>
       </c>
+      <c r="E7" t="s">
+        <v>33</v>
+      </c>
       <c r="G7" t="s">
         <v>4</v>
       </c>
@@ -861,16 +912,16 @@
         <v>6</v>
       </c>
       <c r="Q7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="B8" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>005a</v>
+        <v>005-10</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
@@ -878,6 +929,9 @@
       <c r="D8" t="s">
         <v>15</v>
       </c>
+      <c r="E8" t="s">
+        <v>33</v>
+      </c>
       <c r="G8" t="s">
         <v>4</v>
       </c>
@@ -885,7 +939,7 @@
         <v>4</v>
       </c>
       <c r="I8">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J8">
         <v>2</v>
@@ -905,21 +959,14 @@
       <c r="O8" t="s">
         <v>6</v>
       </c>
-      <c r="P8" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <f>A7+1</f>
-        <v>6</v>
+      <c r="A9" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="B9" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>006</v>
+        <v>005a</v>
       </c>
       <c r="C9" t="s">
         <v>2</v>
@@ -927,6 +974,9 @@
       <c r="D9" t="s">
         <v>15</v>
       </c>
+      <c r="E9" t="s">
+        <v>33</v>
+      </c>
       <c r="G9" t="s">
         <v>4</v>
       </c>
@@ -946,353 +996,376 @@
         <v>4</v>
       </c>
       <c r="M9" s="1">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="N9" t="s">
+        <v>10</v>
+      </c>
+      <c r="O9" t="s">
+        <v>6</v>
+      </c>
+      <c r="P9" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="2" t="str">
+        <f t="shared" ref="B10" si="2">CONCATENATE("00",A10)</f>
+        <v>005a-10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" t="s">
+        <v>4</v>
+      </c>
+      <c r="H10" t="s">
+        <v>4</v>
+      </c>
+      <c r="I10">
+        <v>10</v>
+      </c>
+      <c r="J10">
+        <v>2</v>
+      </c>
+      <c r="K10">
+        <v>2</v>
+      </c>
+      <c r="L10">
+        <v>4</v>
+      </c>
+      <c r="M10" s="1">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="N10" t="s">
+        <v>10</v>
+      </c>
+      <c r="O10" t="s">
+        <v>6</v>
+      </c>
+      <c r="P10" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f>A7+1</f>
+        <v>6</v>
+      </c>
+      <c r="B11" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>006</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" t="s">
+        <v>4</v>
+      </c>
+      <c r="H11" t="s">
+        <v>4</v>
+      </c>
+      <c r="I11">
+        <v>5</v>
+      </c>
+      <c r="J11">
+        <v>2</v>
+      </c>
+      <c r="K11">
+        <v>2</v>
+      </c>
+      <c r="L11">
+        <v>4</v>
+      </c>
+      <c r="M11" s="1">
         <v>3.2000000000000002E-3</v>
       </c>
-      <c r="N9" t="s">
-        <v>10</v>
-      </c>
-      <c r="O9" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="N11" t="s">
+        <v>10</v>
+      </c>
+      <c r="O11" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="B10" s="2" t="str">
+      <c r="B12" s="2" t="str">
         <f t="shared" si="0"/>
         <v>007</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="B11" s="2" t="str">
+      <c r="B13" s="2" t="str">
         <f t="shared" si="0"/>
         <v>008</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="B12" s="2" t="str">
+      <c r="B14" s="2" t="str">
         <f t="shared" si="0"/>
         <v>009</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="B13" s="2" t="str">
-        <f>CONCATENATE("0",A13)</f>
-        <v>010</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-      <c r="B14" s="2" t="str">
-        <f t="shared" ref="B14:B38" si="2">CONCATENATE("0",A14)</f>
-        <v>011</v>
-      </c>
-    </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B15" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>012</v>
+        <f>CONCATENATE("0",A15)</f>
+        <v>010</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B16" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>013</v>
+        <f t="shared" ref="B16:B40" si="3">CONCATENATE("0",A16)</f>
+        <v>011</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B17" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>014</v>
-      </c>
-      <c r="C17" t="s">
-        <v>2</v>
-      </c>
-      <c r="D17" t="s">
-        <v>15</v>
-      </c>
-      <c r="G17" t="s">
-        <v>4</v>
-      </c>
-      <c r="H17" t="s">
-        <v>4</v>
-      </c>
-      <c r="I17">
-        <v>5</v>
-      </c>
-      <c r="J17">
-        <v>2</v>
-      </c>
-      <c r="K17">
-        <v>2</v>
-      </c>
-      <c r="L17">
-        <v>2</v>
-      </c>
-      <c r="M17" s="1">
-        <v>1.6000000000000001E-3</v>
-      </c>
-      <c r="N17" t="s">
-        <v>10</v>
-      </c>
-      <c r="O17" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>22</v>
+        <f t="shared" si="3"/>
+        <v>012</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B18" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>015</v>
-      </c>
-      <c r="C18" t="s">
-        <v>2</v>
-      </c>
-      <c r="D18" t="s">
-        <v>15</v>
-      </c>
-      <c r="G18" t="s">
-        <v>4</v>
-      </c>
-      <c r="H18" t="s">
-        <v>4</v>
-      </c>
-      <c r="I18">
-        <v>5</v>
-      </c>
-      <c r="J18">
-        <v>2</v>
-      </c>
-      <c r="K18">
-        <v>2</v>
-      </c>
-      <c r="L18">
-        <v>8</v>
-      </c>
-      <c r="M18" s="1">
-        <v>1.6000000000000001E-3</v>
-      </c>
-      <c r="N18" t="s">
-        <v>10</v>
-      </c>
-      <c r="O18" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>22</v>
+        <f t="shared" si="3"/>
+        <v>013</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B19" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>016</v>
+        <f t="shared" si="3"/>
+        <v>014</v>
+      </c>
+      <c r="C19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" t="s">
+        <v>33</v>
+      </c>
+      <c r="G19" t="s">
+        <v>4</v>
+      </c>
+      <c r="H19" t="s">
+        <v>4</v>
+      </c>
+      <c r="I19">
+        <v>5</v>
+      </c>
+      <c r="J19">
+        <v>2</v>
+      </c>
+      <c r="K19">
+        <v>2</v>
+      </c>
+      <c r="L19">
+        <v>2</v>
+      </c>
+      <c r="M19" s="1">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="N19" t="s">
+        <v>10</v>
+      </c>
+      <c r="O19" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B20" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>017</v>
+        <f t="shared" si="3"/>
+        <v>015</v>
+      </c>
+      <c r="C20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" t="s">
+        <v>33</v>
+      </c>
+      <c r="G20" t="s">
+        <v>4</v>
+      </c>
+      <c r="H20" t="s">
+        <v>4</v>
+      </c>
+      <c r="I20">
+        <v>5</v>
+      </c>
+      <c r="J20">
+        <v>2</v>
+      </c>
+      <c r="K20">
+        <v>2</v>
+      </c>
+      <c r="L20">
+        <v>8</v>
+      </c>
+      <c r="M20" s="1">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="N20" t="s">
+        <v>10</v>
+      </c>
+      <c r="O20" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B21" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>018</v>
+        <f t="shared" si="3"/>
+        <v>016</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B22" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>019</v>
+        <f t="shared" si="3"/>
+        <v>017</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B23" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>020</v>
+        <f t="shared" si="3"/>
+        <v>018</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="1"/>
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B24" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>021</v>
+        <f t="shared" si="3"/>
+        <v>019</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B25" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>022</v>
+        <f t="shared" si="3"/>
+        <v>020</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="1"/>
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B26" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>023</v>
-      </c>
-      <c r="C26" t="s">
-        <v>2</v>
-      </c>
-      <c r="D26" t="s">
-        <v>24</v>
-      </c>
-      <c r="G26" t="s">
-        <v>4</v>
-      </c>
-      <c r="H26" t="s">
-        <v>4</v>
-      </c>
-      <c r="I26">
-        <v>5</v>
-      </c>
-      <c r="J26">
-        <v>2</v>
-      </c>
-      <c r="K26">
-        <v>2</v>
-      </c>
-      <c r="L26">
-        <v>4</v>
-      </c>
-      <c r="M26" s="1">
-        <v>1.6000000000000001E-3</v>
-      </c>
-      <c r="N26" t="s">
-        <v>10</v>
-      </c>
-      <c r="O26" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>22</v>
+        <f t="shared" si="3"/>
+        <v>021</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="1"/>
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B27" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>024</v>
-      </c>
-      <c r="C27" t="s">
-        <v>2</v>
-      </c>
-      <c r="D27" t="s">
-        <v>23</v>
-      </c>
-      <c r="G27" t="s">
-        <v>4</v>
-      </c>
-      <c r="H27" t="s">
-        <v>4</v>
-      </c>
-      <c r="I27">
-        <v>5</v>
-      </c>
-      <c r="J27">
-        <v>2</v>
-      </c>
-      <c r="K27">
-        <v>2</v>
-      </c>
-      <c r="L27">
-        <v>4</v>
-      </c>
-      <c r="M27" s="1">
-        <v>1.6000000000000001E-3</v>
-      </c>
-      <c r="N27" t="s">
-        <v>10</v>
-      </c>
-      <c r="O27" t="s">
-        <v>6</v>
+        <f t="shared" si="3"/>
+        <v>022</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B28" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>025</v>
+        <f t="shared" si="3"/>
+        <v>023</v>
       </c>
       <c r="C28" t="s">
         <v>2</v>
       </c>
       <c r="D28" t="s">
-        <v>18</v>
+        <v>23</v>
+      </c>
+      <c r="E28" t="s">
+        <v>33</v>
       </c>
       <c r="G28" t="s">
         <v>4</v>
@@ -1322,23 +1395,26 @@
         <v>6</v>
       </c>
       <c r="Q28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="1"/>
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B29" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>026</v>
+        <f t="shared" si="3"/>
+        <v>024</v>
       </c>
       <c r="C29" t="s">
         <v>2</v>
       </c>
       <c r="D29" t="s">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c r="E29" t="s">
+        <v>33</v>
       </c>
       <c r="G29" t="s">
         <v>4</v>
@@ -1367,654 +1443,1175 @@
       <c r="O29" t="s">
         <v>6</v>
       </c>
-      <c r="Q29" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" si="1"/>
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B30" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>027</v>
+        <f t="shared" si="3"/>
+        <v>025</v>
+      </c>
+      <c r="C30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D30" t="s">
+        <v>17</v>
+      </c>
+      <c r="E30" t="s">
+        <v>33</v>
+      </c>
+      <c r="G30" t="s">
+        <v>4</v>
+      </c>
+      <c r="H30" t="s">
+        <v>4</v>
+      </c>
+      <c r="I30">
+        <v>5</v>
+      </c>
+      <c r="J30">
+        <v>2</v>
+      </c>
+      <c r="K30">
+        <v>2</v>
+      </c>
+      <c r="L30">
+        <v>4</v>
+      </c>
+      <c r="M30" s="1">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="N30" t="s">
+        <v>10</v>
+      </c>
+      <c r="O30" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B31" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>028</v>
+        <f t="shared" si="3"/>
+        <v>026</v>
+      </c>
+      <c r="C31" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E31" t="s">
+        <v>33</v>
+      </c>
+      <c r="G31" t="s">
+        <v>4</v>
+      </c>
+      <c r="H31" t="s">
+        <v>4</v>
+      </c>
+      <c r="I31">
+        <v>5</v>
+      </c>
+      <c r="J31">
+        <v>2</v>
+      </c>
+      <c r="K31">
+        <v>2</v>
+      </c>
+      <c r="L31">
+        <v>4</v>
+      </c>
+      <c r="M31" s="1">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="N31" t="s">
+        <v>10</v>
+      </c>
+      <c r="O31" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" si="1"/>
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B32" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>029</v>
+        <f t="shared" si="3"/>
+        <v>027</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B33" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>030</v>
+        <f t="shared" si="3"/>
+        <v>028</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B34" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>031</v>
+        <f t="shared" si="3"/>
+        <v>029</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B35" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>032</v>
+        <f t="shared" si="3"/>
+        <v>030</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="shared" si="1"/>
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B36" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>033</v>
+        <f t="shared" si="3"/>
+        <v>031</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37">
         <f t="shared" si="1"/>
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B37" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>034</v>
+        <f t="shared" si="3"/>
+        <v>032</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B38" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>035</v>
-      </c>
-      <c r="C38" t="s">
-        <v>2</v>
-      </c>
-      <c r="D38" t="s">
-        <v>19</v>
-      </c>
-      <c r="G38" t="s">
-        <v>4</v>
-      </c>
-      <c r="H38" t="s">
-        <v>4</v>
-      </c>
-      <c r="I38">
-        <v>5</v>
-      </c>
-      <c r="J38">
-        <v>2</v>
-      </c>
-      <c r="K38">
-        <v>2</v>
-      </c>
-      <c r="L38">
-        <v>4</v>
-      </c>
-      <c r="M38" s="1">
-        <v>1.6000000000000001E-3</v>
-      </c>
-      <c r="N38" t="s">
-        <v>10</v>
-      </c>
-      <c r="O38" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q38" t="s">
-        <v>22</v>
+        <f t="shared" si="3"/>
+        <v>033</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39">
         <f t="shared" si="1"/>
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B39" s="2" t="str">
-        <f t="shared" ref="B39:B53" si="3">CONCATENATE("0",A39)</f>
-        <v>036</v>
-      </c>
-      <c r="C39" t="s">
-        <v>2</v>
-      </c>
-      <c r="D39" t="s">
-        <v>25</v>
-      </c>
-      <c r="G39" t="s">
-        <v>4</v>
-      </c>
-      <c r="H39" t="s">
-        <v>4</v>
-      </c>
-      <c r="I39">
-        <v>5</v>
-      </c>
-      <c r="J39">
-        <v>2</v>
-      </c>
-      <c r="K39">
-        <v>2</v>
-      </c>
-      <c r="L39">
-        <v>4</v>
-      </c>
-      <c r="M39" s="1">
-        <v>1.6000000000000001E-3</v>
-      </c>
-      <c r="N39" t="s">
-        <v>10</v>
-      </c>
-      <c r="O39" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q39" t="s">
-        <v>22</v>
+        <f t="shared" si="3"/>
+        <v>034</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40">
         <f t="shared" si="1"/>
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B40" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>037</v>
+        <v>035</v>
+      </c>
+      <c r="C40" t="s">
+        <v>2</v>
+      </c>
+      <c r="D40" t="s">
+        <v>18</v>
+      </c>
+      <c r="E40" t="s">
+        <v>33</v>
+      </c>
+      <c r="G40" t="s">
+        <v>4</v>
+      </c>
+      <c r="H40" t="s">
+        <v>4</v>
+      </c>
+      <c r="I40">
+        <v>5</v>
+      </c>
+      <c r="J40">
+        <v>2</v>
+      </c>
+      <c r="K40">
+        <v>2</v>
+      </c>
+      <c r="L40">
+        <v>4</v>
+      </c>
+      <c r="M40" s="1">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="N40" t="s">
+        <v>10</v>
+      </c>
+      <c r="O40" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41">
         <f t="shared" si="1"/>
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B41" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>038</v>
+        <f t="shared" ref="B41:B55" si="4">CONCATENATE("0",A41)</f>
+        <v>036</v>
+      </c>
+      <c r="C41" t="s">
+        <v>2</v>
+      </c>
+      <c r="D41" t="s">
+        <v>24</v>
+      </c>
+      <c r="E41" t="s">
+        <v>33</v>
+      </c>
+      <c r="G41" t="s">
+        <v>4</v>
+      </c>
+      <c r="H41" t="s">
+        <v>4</v>
+      </c>
+      <c r="I41">
+        <v>5</v>
+      </c>
+      <c r="J41">
+        <v>2</v>
+      </c>
+      <c r="K41">
+        <v>2</v>
+      </c>
+      <c r="L41">
+        <v>4</v>
+      </c>
+      <c r="M41" s="1">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="N41" t="s">
+        <v>10</v>
+      </c>
+      <c r="O41" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42">
         <f t="shared" si="1"/>
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B42" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>039</v>
+        <f t="shared" si="4"/>
+        <v>037</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B43" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>040</v>
+        <f t="shared" si="4"/>
+        <v>038</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44">
         <f t="shared" si="1"/>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B44" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>041</v>
+        <f t="shared" si="4"/>
+        <v>039</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45">
         <f t="shared" si="1"/>
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B45" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>042</v>
+        <f t="shared" si="4"/>
+        <v>040</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46">
         <f t="shared" si="1"/>
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B46" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>043</v>
+        <f t="shared" si="4"/>
+        <v>041</v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47">
         <f t="shared" si="1"/>
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B47" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>044</v>
+        <f t="shared" si="4"/>
+        <v>042</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48">
         <f t="shared" si="1"/>
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B48" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>045</v>
+        <f t="shared" si="4"/>
+        <v>043</v>
       </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49">
         <f t="shared" si="1"/>
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B49" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>046</v>
-      </c>
-      <c r="C49" t="s">
-        <v>2</v>
-      </c>
-      <c r="D49" t="s">
-        <v>26</v>
-      </c>
-      <c r="G49" t="s">
-        <v>4</v>
-      </c>
-      <c r="H49" t="s">
-        <v>4</v>
-      </c>
-      <c r="I49">
-        <v>5</v>
-      </c>
-      <c r="J49">
-        <v>2</v>
-      </c>
-      <c r="K49">
-        <v>2</v>
-      </c>
-      <c r="L49">
-        <v>4</v>
-      </c>
-      <c r="M49" s="1">
-        <v>1.6000000000000001E-3</v>
-      </c>
-      <c r="N49" t="s">
-        <v>10</v>
-      </c>
-      <c r="O49" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q49" t="s">
-        <v>22</v>
+        <f t="shared" si="4"/>
+        <v>044</v>
       </c>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50">
         <f t="shared" si="1"/>
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B50" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>047</v>
-      </c>
-      <c r="C50" t="s">
-        <v>2</v>
-      </c>
-      <c r="D50" t="s">
-        <v>27</v>
-      </c>
-      <c r="G50" t="s">
-        <v>4</v>
-      </c>
-      <c r="H50" t="s">
-        <v>4</v>
-      </c>
-      <c r="I50">
-        <v>5</v>
-      </c>
-      <c r="J50">
-        <v>2</v>
-      </c>
-      <c r="K50">
-        <v>2</v>
-      </c>
-      <c r="L50">
-        <v>4</v>
-      </c>
-      <c r="M50" s="1">
-        <v>1.6000000000000001E-3</v>
-      </c>
-      <c r="N50" t="s">
-        <v>10</v>
-      </c>
-      <c r="O50" t="s">
-        <v>6</v>
+        <f t="shared" si="4"/>
+        <v>045</v>
       </c>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51">
         <f t="shared" si="1"/>
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B51" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>048</v>
+        <f t="shared" si="4"/>
+        <v>046</v>
+      </c>
+      <c r="C51" t="s">
+        <v>2</v>
+      </c>
+      <c r="D51" t="s">
+        <v>25</v>
+      </c>
+      <c r="E51" t="s">
+        <v>33</v>
+      </c>
+      <c r="G51" t="s">
+        <v>4</v>
+      </c>
+      <c r="H51" t="s">
+        <v>4</v>
+      </c>
+      <c r="I51">
+        <v>5</v>
+      </c>
+      <c r="J51">
+        <v>2</v>
+      </c>
+      <c r="K51">
+        <v>2</v>
+      </c>
+      <c r="L51">
+        <v>4</v>
+      </c>
+      <c r="M51" s="1">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="N51" t="s">
+        <v>10</v>
+      </c>
+      <c r="O51" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52">
         <f t="shared" si="1"/>
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B52" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>049</v>
+        <f t="shared" si="4"/>
+        <v>047</v>
+      </c>
+      <c r="C52" t="s">
+        <v>2</v>
+      </c>
+      <c r="D52" t="s">
+        <v>26</v>
+      </c>
+      <c r="E52" t="s">
+        <v>33</v>
+      </c>
+      <c r="G52" t="s">
+        <v>4</v>
+      </c>
+      <c r="H52" t="s">
+        <v>4</v>
+      </c>
+      <c r="I52">
+        <v>5</v>
+      </c>
+      <c r="J52">
+        <v>2</v>
+      </c>
+      <c r="K52">
+        <v>2</v>
+      </c>
+      <c r="L52">
+        <v>4</v>
+      </c>
+      <c r="M52" s="1">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="N52" t="s">
+        <v>10</v>
+      </c>
+      <c r="O52" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53">
         <f t="shared" si="1"/>
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B53" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>050</v>
+        <f t="shared" si="4"/>
+        <v>048</v>
       </c>
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54">
         <f t="shared" si="1"/>
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B54" s="2" t="str">
-        <f t="shared" ref="B54:B72" si="4">CONCATENATE("0",A54)</f>
-        <v>051</v>
+        <f t="shared" si="4"/>
+        <v>049</v>
       </c>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55">
         <f t="shared" si="1"/>
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B55" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>052</v>
+        <v>050</v>
       </c>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56">
         <f t="shared" si="1"/>
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B56" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>053</v>
+        <f t="shared" ref="B56:B77" si="5">CONCATENATE("0",A56)</f>
+        <v>051</v>
       </c>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A57">
         <f t="shared" si="1"/>
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B57" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>054</v>
+        <f t="shared" si="5"/>
+        <v>052</v>
       </c>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A58">
         <f t="shared" si="1"/>
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B58" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>055</v>
-      </c>
-      <c r="C58" t="s">
-        <v>2</v>
-      </c>
-      <c r="D58" t="s">
-        <v>31</v>
-      </c>
-      <c r="G58" t="s">
-        <v>4</v>
-      </c>
-      <c r="H58" t="s">
-        <v>4</v>
-      </c>
-      <c r="I58">
-        <v>10</v>
-      </c>
-      <c r="J58">
-        <v>2</v>
-      </c>
-      <c r="K58">
-        <v>2</v>
-      </c>
-      <c r="L58">
-        <v>4</v>
-      </c>
-      <c r="M58" s="1">
-        <v>1.6000000000000001E-3</v>
-      </c>
-      <c r="N58" t="s">
-        <v>10</v>
-      </c>
-      <c r="O58" t="s">
-        <v>6</v>
-      </c>
-      <c r="P58" t="s">
-        <v>30</v>
+        <f t="shared" si="5"/>
+        <v>053</v>
       </c>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59">
         <f t="shared" si="1"/>
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B59" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>056</v>
-      </c>
-      <c r="C59" t="s">
-        <v>2</v>
-      </c>
-      <c r="D59" t="s">
-        <v>31</v>
-      </c>
-      <c r="E59">
-        <v>0.1</v>
-      </c>
-      <c r="G59" t="s">
-        <v>4</v>
-      </c>
-      <c r="H59" t="s">
-        <v>4</v>
-      </c>
-      <c r="I59">
-        <v>10</v>
-      </c>
-      <c r="J59">
-        <v>2</v>
-      </c>
-      <c r="K59">
-        <v>2</v>
-      </c>
-      <c r="L59">
-        <v>4</v>
-      </c>
-      <c r="M59" s="1">
-        <v>1.6000000000000001E-3</v>
-      </c>
-      <c r="N59" t="s">
-        <v>10</v>
-      </c>
-      <c r="O59" t="s">
-        <v>6</v>
-      </c>
-      <c r="P59" t="s">
-        <v>30</v>
+        <f t="shared" si="5"/>
+        <v>054</v>
       </c>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60">
         <f t="shared" si="1"/>
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B60" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>057</v>
+        <f t="shared" si="5"/>
+        <v>055</v>
+      </c>
+      <c r="C60" t="s">
+        <v>2</v>
+      </c>
+      <c r="D60" t="s">
+        <v>15</v>
+      </c>
+      <c r="E60" t="s">
+        <v>34</v>
+      </c>
+      <c r="G60" t="s">
+        <v>4</v>
+      </c>
+      <c r="H60" t="s">
+        <v>4</v>
+      </c>
+      <c r="I60">
+        <v>10</v>
+      </c>
+      <c r="J60">
+        <v>2</v>
+      </c>
+      <c r="K60">
+        <v>2</v>
+      </c>
+      <c r="L60">
+        <v>4</v>
+      </c>
+      <c r="M60" s="1">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="N60" t="s">
+        <v>10</v>
+      </c>
+      <c r="O60" t="s">
+        <v>6</v>
+      </c>
+      <c r="P60" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q60" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A61">
-        <f t="shared" si="1"/>
-        <v>58</v>
+      <c r="A61" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="B61" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>058</v>
+        <f t="shared" ref="B61:B62" si="6">CONCATENATE("0",A61)</f>
+        <v>055a</v>
+      </c>
+      <c r="C61" t="s">
+        <v>2</v>
+      </c>
+      <c r="D61" t="s">
+        <v>15</v>
+      </c>
+      <c r="E61" t="s">
+        <v>40</v>
+      </c>
+      <c r="G61" t="s">
+        <v>4</v>
+      </c>
+      <c r="H61" t="s">
+        <v>4</v>
+      </c>
+      <c r="I61">
+        <v>10</v>
+      </c>
+      <c r="J61">
+        <v>2</v>
+      </c>
+      <c r="K61">
+        <v>2</v>
+      </c>
+      <c r="L61">
+        <v>4</v>
+      </c>
+      <c r="M61" s="1">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="N61" t="s">
+        <v>10</v>
+      </c>
+      <c r="O61" t="s">
+        <v>6</v>
+      </c>
+      <c r="P61" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q61" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A62">
-        <f t="shared" si="1"/>
-        <v>59</v>
+      <c r="A62" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="B62" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>059</v>
+        <f t="shared" si="6"/>
+        <v>055b</v>
+      </c>
+      <c r="C62" t="s">
+        <v>2</v>
+      </c>
+      <c r="D62" t="s">
+        <v>15</v>
+      </c>
+      <c r="E62" t="s">
+        <v>43</v>
+      </c>
+      <c r="G62" t="s">
+        <v>4</v>
+      </c>
+      <c r="H62" t="s">
+        <v>4</v>
+      </c>
+      <c r="I62">
+        <v>10</v>
+      </c>
+      <c r="J62">
+        <v>2</v>
+      </c>
+      <c r="K62">
+        <v>2</v>
+      </c>
+      <c r="L62">
+        <v>4</v>
+      </c>
+      <c r="M62" s="1">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="N62" t="s">
+        <v>10</v>
+      </c>
+      <c r="O62" t="s">
+        <v>6</v>
+      </c>
+      <c r="P62" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q62" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A63">
-        <f t="shared" si="1"/>
-        <v>60</v>
+      <c r="A63" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="B63" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>060</v>
+        <f t="shared" ref="B63" si="7">CONCATENATE("0",A63)</f>
+        <v>055c</v>
+      </c>
+      <c r="C63" t="s">
+        <v>2</v>
+      </c>
+      <c r="D63" t="s">
+        <v>15</v>
+      </c>
+      <c r="E63" t="s">
+        <v>44</v>
+      </c>
+      <c r="G63" t="s">
+        <v>4</v>
+      </c>
+      <c r="H63" t="s">
+        <v>4</v>
+      </c>
+      <c r="I63">
+        <v>10</v>
+      </c>
+      <c r="J63">
+        <v>2</v>
+      </c>
+      <c r="K63">
+        <v>2</v>
+      </c>
+      <c r="L63">
+        <v>4</v>
+      </c>
+      <c r="M63" s="1">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="N63" t="s">
+        <v>10</v>
+      </c>
+      <c r="O63" t="s">
+        <v>6</v>
+      </c>
+      <c r="P63" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q63" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A64">
+        <f>A60+1</f>
+        <v>56</v>
+      </c>
+      <c r="B64" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>056</v>
+      </c>
+      <c r="M64" s="1"/>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <f t="shared" si="1"/>
+        <v>57</v>
+      </c>
+      <c r="B65" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>057</v>
+      </c>
+      <c r="C65" t="s">
+        <v>2</v>
+      </c>
+      <c r="D65" t="s">
+        <v>15</v>
+      </c>
+      <c r="E65" t="s">
+        <v>36</v>
+      </c>
+      <c r="G65" t="s">
+        <v>4</v>
+      </c>
+      <c r="H65" t="s">
+        <v>4</v>
+      </c>
+      <c r="I65">
+        <v>10</v>
+      </c>
+      <c r="J65">
+        <v>2</v>
+      </c>
+      <c r="K65">
+        <v>2</v>
+      </c>
+      <c r="L65">
+        <v>4</v>
+      </c>
+      <c r="M65" s="1">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="N65" t="s">
+        <v>10</v>
+      </c>
+      <c r="O65" t="s">
+        <v>6</v>
+      </c>
+      <c r="P65" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q65" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <f t="shared" si="1"/>
+        <v>58</v>
+      </c>
+      <c r="B66" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>058</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <f t="shared" si="1"/>
+        <v>59</v>
+      </c>
+      <c r="B67" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>059</v>
+      </c>
+      <c r="M67" s="1"/>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="B68" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>060</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A69">
         <f t="shared" si="1"/>
         <v>61</v>
       </c>
-      <c r="B64" s="2" t="str">
-        <f t="shared" si="4"/>
+      <c r="B69" s="2" t="str">
+        <f t="shared" si="5"/>
         <v>061</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A70">
         <f t="shared" si="1"/>
         <v>62</v>
       </c>
-      <c r="B65" s="2" t="str">
-        <f t="shared" si="4"/>
+      <c r="B70" s="2" t="str">
+        <f t="shared" si="5"/>
         <v>062</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66">
+      <c r="C70" t="s">
+        <v>2</v>
+      </c>
+      <c r="D70" t="s">
+        <v>15</v>
+      </c>
+      <c r="E70" t="s">
+        <v>35</v>
+      </c>
+      <c r="G70" t="s">
+        <v>4</v>
+      </c>
+      <c r="H70" t="s">
+        <v>4</v>
+      </c>
+      <c r="I70">
+        <v>10</v>
+      </c>
+      <c r="J70">
+        <v>2</v>
+      </c>
+      <c r="K70">
+        <v>2</v>
+      </c>
+      <c r="L70">
+        <v>4</v>
+      </c>
+      <c r="M70" s="1">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="N70" t="s">
+        <v>10</v>
+      </c>
+      <c r="O70" t="s">
+        <v>6</v>
+      </c>
+      <c r="P70" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q70" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A71">
         <f t="shared" si="1"/>
         <v>63</v>
       </c>
-      <c r="B66" s="2" t="str">
-        <f t="shared" si="4"/>
+      <c r="B71" s="2" t="str">
+        <f t="shared" si="5"/>
         <v>063</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A72">
         <f t="shared" si="1"/>
         <v>64</v>
       </c>
-      <c r="B67" s="2" t="str">
-        <f t="shared" si="4"/>
+      <c r="B72" s="2" t="str">
+        <f t="shared" si="5"/>
         <v>064</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68">
-        <f t="shared" ref="A68:A72" si="5">A67+1</f>
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <f t="shared" ref="A73:A84" si="8">A72+1</f>
         <v>65</v>
       </c>
-      <c r="B68" s="2" t="str">
-        <f t="shared" si="4"/>
+      <c r="B73" s="2" t="str">
+        <f t="shared" si="5"/>
         <v>065</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69">
+      <c r="C73" t="s">
+        <v>2</v>
+      </c>
+      <c r="D73" t="s">
+        <v>15</v>
+      </c>
+      <c r="E73" t="s">
+        <v>33</v>
+      </c>
+      <c r="F73" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="G73" t="s">
+        <v>4</v>
+      </c>
+      <c r="H73" t="s">
+        <v>4</v>
+      </c>
+      <c r="I73">
+        <v>10</v>
+      </c>
+      <c r="J73">
+        <v>2</v>
+      </c>
+      <c r="K73">
+        <v>2</v>
+      </c>
+      <c r="L73">
+        <v>4</v>
+      </c>
+      <c r="M73" s="1">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="N73" t="s">
+        <v>10</v>
+      </c>
+      <c r="O73" t="s">
+        <v>6</v>
+      </c>
+      <c r="P73" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q73" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <f t="shared" si="8"/>
+        <v>66</v>
+      </c>
+      <c r="B74" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>66</v>
-      </c>
-      <c r="B69" s="2" t="str">
-        <f t="shared" si="4"/>
         <v>066</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <f t="shared" si="8"/>
+        <v>67</v>
+      </c>
+      <c r="B75" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>67</v>
-      </c>
-      <c r="B70" s="2" t="str">
-        <f t="shared" si="4"/>
         <v>067</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71">
+      <c r="C75" t="s">
+        <v>2</v>
+      </c>
+      <c r="D75" t="s">
+        <v>15</v>
+      </c>
+      <c r="E75" t="s">
+        <v>33</v>
+      </c>
+      <c r="F75" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="G75" t="s">
+        <v>4</v>
+      </c>
+      <c r="H75" t="s">
+        <v>4</v>
+      </c>
+      <c r="I75">
+        <v>10</v>
+      </c>
+      <c r="J75">
+        <v>2</v>
+      </c>
+      <c r="K75">
+        <v>2</v>
+      </c>
+      <c r="L75">
+        <v>4</v>
+      </c>
+      <c r="M75" s="1">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="N75" t="s">
+        <v>10</v>
+      </c>
+      <c r="O75" t="s">
+        <v>6</v>
+      </c>
+      <c r="P75" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q75" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <f t="shared" si="8"/>
+        <v>68</v>
+      </c>
+      <c r="B76" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>68</v>
-      </c>
-      <c r="B71" s="2" t="str">
-        <f t="shared" si="4"/>
         <v>068</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <f t="shared" si="8"/>
+        <v>69</v>
+      </c>
+      <c r="B77" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>69</v>
-      </c>
-      <c r="B72" s="2" t="str">
-        <f t="shared" si="4"/>
         <v>069</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <f t="shared" si="8"/>
+        <v>70</v>
+      </c>
+      <c r="B78" s="2" t="str">
+        <f t="shared" ref="B78:B84" si="9">CONCATENATE("0",A78)</f>
+        <v>070</v>
+      </c>
+      <c r="C78" t="s">
+        <v>2</v>
+      </c>
+      <c r="D78" t="s">
+        <v>15</v>
+      </c>
+      <c r="E78" t="s">
+        <v>33</v>
+      </c>
+      <c r="F78" s="1">
+        <v>10</v>
+      </c>
+      <c r="G78" t="s">
+        <v>4</v>
+      </c>
+      <c r="H78" t="s">
+        <v>4</v>
+      </c>
+      <c r="I78">
+        <v>10</v>
+      </c>
+      <c r="J78">
+        <v>2</v>
+      </c>
+      <c r="K78">
+        <v>2</v>
+      </c>
+      <c r="L78">
+        <v>4</v>
+      </c>
+      <c r="M78" s="1">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="N78" t="s">
+        <v>10</v>
+      </c>
+      <c r="O78" t="s">
+        <v>6</v>
+      </c>
+      <c r="P78" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q78" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <f t="shared" si="8"/>
+        <v>71</v>
+      </c>
+      <c r="B79" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>071</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <f t="shared" si="8"/>
+        <v>72</v>
+      </c>
+      <c r="B80" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>072</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <f t="shared" si="8"/>
+        <v>73</v>
+      </c>
+      <c r="B81" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>073</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <f t="shared" si="8"/>
+        <v>74</v>
+      </c>
+      <c r="B82" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>074</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <f t="shared" si="8"/>
+        <v>75</v>
+      </c>
+      <c r="B83" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>075</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <f t="shared" si="8"/>
+        <v>76</v>
+      </c>
+      <c r="B84" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>076</v>
       </c>
     </row>
   </sheetData>

</xml_diff>